<commit_message>
Full Project and Dashboard
</commit_message>
<xml_diff>
--- a/Data Cleaning Excel Tutorial.xlsx
+++ b/Data Cleaning Excel Tutorial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analysis\Excel\Playlist of Alex The Analyst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC30E6-74AA-4FA4-8BCE-6BE30C48FA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F06082-073C-425E-94CC-EA5DAA42878B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1144,7 +1144,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Data Analysis Projcet Using Excel 2
</commit_message>
<xml_diff>
--- a/Data Cleaning Excel Tutorial.xlsx
+++ b/Data Cleaning Excel Tutorial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analysis\Excel\Playlist of Alex The Analyst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F06082-073C-425E-94CC-EA5DAA42878B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55018DDF-6956-4A86-9793-F43A8453B20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1144,7 +1144,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>